<commit_message>
changed beihai start month from 6 to 4
</commit_message>
<xml_diff>
--- a/dataset/21_ROIs.xlsx
+++ b/dataset/21_ROIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97DF8DC-B682-4A01-8A1A-7F906EC12628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCCE0B1-0DD6-450F-88C9-F2B7438C30DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROIs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="112">
   <si>
     <t>name</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>[[[-0.486832, 39.351813], [-0.486832, 39.553816], [-0.300751, 39.553816], [-0.300751, 39.351813], [-0.486832, 39.351813]]]</t>
+  </si>
+  <si>
+    <t>('2021-04-07','2021-05-07')</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1053,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1282,7 +1285,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>26</v>
@@ -1332,7 +1335,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>26</v>
@@ -1382,7 +1385,7 @@
         <v>30</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
chongqing mont changed from 6 to 4
</commit_message>
<xml_diff>
--- a/dataset/21_ROIs.xlsx
+++ b/dataset/21_ROIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCCE0B1-0DD6-450F-88C9-F2B7438C30DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF6C3A9-DD5D-4B19-AB98-89986BAB0A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1053,7 +1053,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D16" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1385,7 +1385,7 @@
         <v>30</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>26</v>
@@ -1843,7 +1843,7 @@
         <v>50</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>26</v>
@@ -1893,7 +1893,7 @@
         <v>52</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>26</v>
@@ -30080,17 +30080,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:K1000">
-    <cfRule type="expression" dxfId="47" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$K2="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:K1000">
-    <cfRule type="expression" dxfId="46" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$K2="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:K1000">
-    <cfRule type="expression" dxfId="45" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$K2="main"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30107,17 +30107,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26:J27 F28:H31">
-    <cfRule type="expression" dxfId="44" priority="5">
+    <cfRule type="expression" dxfId="47" priority="5">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26:J27 F28:H31">
-    <cfRule type="expression" dxfId="43" priority="6">
+    <cfRule type="expression" dxfId="46" priority="6">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26:J27 F28:H31">
-    <cfRule type="expression" dxfId="42" priority="7">
+    <cfRule type="expression" dxfId="45" priority="7">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30134,212 +30134,212 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32:H38 F40:H41">
-    <cfRule type="expression" dxfId="41" priority="9">
+    <cfRule type="expression" dxfId="44" priority="9">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32:H38 F40:H41">
-    <cfRule type="expression" dxfId="40" priority="10">
+    <cfRule type="expression" dxfId="43" priority="10">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32:H38 F40:H41">
-    <cfRule type="expression" dxfId="39" priority="11">
+    <cfRule type="expression" dxfId="42" priority="11">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39:H39">
-    <cfRule type="expression" dxfId="38" priority="12">
+    <cfRule type="expression" dxfId="41" priority="12">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39:H39">
-    <cfRule type="expression" dxfId="37" priority="13">
+    <cfRule type="expression" dxfId="40" priority="13">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39:H39">
-    <cfRule type="expression" dxfId="36" priority="14">
+    <cfRule type="expression" dxfId="39" priority="14">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:H42">
-    <cfRule type="expression" dxfId="35" priority="15">
+    <cfRule type="expression" dxfId="38" priority="15">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:H42">
-    <cfRule type="expression" dxfId="34" priority="16">
+    <cfRule type="expression" dxfId="37" priority="16">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:H42">
-    <cfRule type="expression" dxfId="33" priority="17">
+    <cfRule type="expression" dxfId="36" priority="17">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:H42">
-    <cfRule type="expression" dxfId="32" priority="18">
+    <cfRule type="expression" dxfId="35" priority="18">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:H42">
-    <cfRule type="expression" dxfId="31" priority="19">
+    <cfRule type="expression" dxfId="34" priority="19">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:H42">
-    <cfRule type="expression" dxfId="30" priority="20">
+    <cfRule type="expression" dxfId="33" priority="20">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:H43">
-    <cfRule type="expression" dxfId="29" priority="21">
+    <cfRule type="expression" dxfId="32" priority="21">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:H43">
-    <cfRule type="expression" dxfId="28" priority="22">
+    <cfRule type="expression" dxfId="31" priority="22">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:H43">
-    <cfRule type="expression" dxfId="27" priority="23">
+    <cfRule type="expression" dxfId="30" priority="23">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:H43">
-    <cfRule type="expression" dxfId="26" priority="24">
+    <cfRule type="expression" dxfId="29" priority="24">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:H43">
-    <cfRule type="expression" dxfId="25" priority="25">
+    <cfRule type="expression" dxfId="28" priority="25">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:H43">
-    <cfRule type="expression" dxfId="24" priority="26">
+    <cfRule type="expression" dxfId="27" priority="26">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="23" priority="27">
+    <cfRule type="expression" dxfId="26" priority="27">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="22" priority="28">
+    <cfRule type="expression" dxfId="25" priority="28">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="21" priority="29">
+    <cfRule type="expression" dxfId="24" priority="29">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="20" priority="30">
+    <cfRule type="expression" dxfId="23" priority="30">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="19" priority="31">
+    <cfRule type="expression" dxfId="22" priority="31">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="18" priority="32">
+    <cfRule type="expression" dxfId="21" priority="32">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="17" priority="33">
+    <cfRule type="expression" dxfId="20" priority="33">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="16" priority="34">
+    <cfRule type="expression" dxfId="19" priority="34">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="15" priority="35">
+    <cfRule type="expression" dxfId="18" priority="35">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="14" priority="36">
+    <cfRule type="expression" dxfId="17" priority="36">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="13" priority="37">
+    <cfRule type="expression" dxfId="16" priority="37">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="12" priority="38">
+    <cfRule type="expression" dxfId="15" priority="38">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="11" priority="39">
+    <cfRule type="expression" dxfId="14" priority="39">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="10" priority="40">
+    <cfRule type="expression" dxfId="13" priority="40">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="9" priority="41">
+    <cfRule type="expression" dxfId="12" priority="41">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="8" priority="42">
+    <cfRule type="expression" dxfId="11" priority="42">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="7" priority="43">
+    <cfRule type="expression" dxfId="10" priority="43">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="6" priority="44">
+    <cfRule type="expression" dxfId="9" priority="44">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="5" priority="45">
+    <cfRule type="expression" dxfId="8" priority="45">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="4" priority="46">
+    <cfRule type="expression" dxfId="7" priority="46">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="3" priority="47">
+    <cfRule type="expression" dxfId="6" priority="47">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="2" priority="48">
+    <cfRule type="expression" dxfId="5" priority="48">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="1" priority="49">
+    <cfRule type="expression" dxfId="4" priority="49">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="0" priority="50">
+    <cfRule type="expression" dxfId="3" priority="50">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
dubai day_span changed from 0 to 20
</commit_message>
<xml_diff>
--- a/dataset/21_ROIs.xlsx
+++ b/dataset/21_ROIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF6C3A9-DD5D-4B19-AB98-89986BAB0A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85879C43-02FB-4E23-BE06-205D643BA4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1053,7 +1053,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:D17"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2111,7 +2111,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="4">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>17</v>
@@ -2161,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="4">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>20</v>
@@ -2211,7 +2211,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="4">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
hongcong_adj from moth from 6 to 4
</commit_message>
<xml_diff>
--- a/dataset/21_ROIs.xlsx
+++ b/dataset/21_ROIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85879C43-02FB-4E23-BE06-205D643BA4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B6F76F-C7CC-4E7D-8537-08C3306F7F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1053,7 +1053,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2295,7 +2295,7 @@
         <v>68</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
milano moth from 6 to 4
</commit_message>
<xml_diff>
--- a/dataset/21_ROIs.xlsx
+++ b/dataset/21_ROIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B6F76F-C7CC-4E7D-8537-08C3306F7F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11EF73F-9862-48D6-9649-A65A6EF610BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1052,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2447,7 +2447,7 @@
         <v>75</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>15</v>
@@ -2497,7 +2497,7 @@
         <v>77</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
mumbai moth from 6 to 4
</commit_message>
<xml_diff>
--- a/dataset/21_ROIs.xlsx
+++ b/dataset/21_ROIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11EF73F-9862-48D6-9649-A65A6EF610BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4886B46-D24A-4D85-9E4D-F140443417AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1053,7 +1053,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2647,7 +2647,7 @@
         <v>83</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>15</v>
@@ -2697,7 +2697,7 @@
         <v>85</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
max clouf from 2 to 1 for hongkong
</commit_message>
<xml_diff>
--- a/dataset/21_ROIs.xlsx
+++ b/dataset/21_ROIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DEA98E-B30B-420C-975D-6AE88E2C93C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06760CD7-AC31-4EC6-880D-C059F7A40185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="118">
   <si>
     <t>name</t>
   </si>
@@ -358,9 +358,6 @@
   </si>
   <si>
     <t>[[[-0.486832, 39.351813], [-0.486832, 39.553816], [-0.300751, 39.553816], [-0.300751, 39.351813], [-0.486832, 39.351813]]]</t>
-  </si>
-  <si>
-    <t>('2021-04-07','2021-05-07')</t>
   </si>
   <si>
     <t>('2021-07-07','2021-08-07')</t>
@@ -1161,7 +1158,7 @@
   <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1212,7 +1209,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>10</v>
@@ -1267,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>17</v>
@@ -1320,7 +1317,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>20</v>
@@ -1343,7 +1340,7 @@
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="4">
         <v>21</v>
@@ -1373,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>17</v>
@@ -1396,7 +1393,7 @@
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="4">
         <v>21</v>
@@ -1426,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>20</v>
@@ -1479,7 +1476,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>23</v>
@@ -1532,7 +1529,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>17</v>
@@ -1585,7 +1582,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>20</v>
@@ -1638,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>23</v>
@@ -1691,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>17</v>
@@ -1744,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>23</v>
@@ -1797,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>17</v>
@@ -1852,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>20</v>
@@ -1907,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>17</v>
@@ -1962,7 +1959,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>20</v>
@@ -2017,7 +2014,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L16" s="6" t="s">
         <v>17</v>
@@ -2070,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L17" s="6" t="s">
         <v>20</v>
@@ -2123,7 +2120,7 @@
         <v>18</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L18" s="6" t="s">
         <v>17</v>
@@ -2176,7 +2173,7 @@
         <v>18</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L19" s="6" t="s">
         <v>23</v>
@@ -2229,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L20" s="6" t="s">
         <v>17</v>
@@ -2282,7 +2279,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L21" s="6" t="s">
         <v>20</v>
@@ -2335,7 +2332,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L22" s="6" t="s">
         <v>23</v>
@@ -2388,7 +2385,7 @@
         <v>18</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L23" s="6" t="s">
         <v>17</v>
@@ -2441,7 +2438,7 @@
         <v>18</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L24" s="6" t="s">
         <v>20</v>
@@ -2494,7 +2491,7 @@
         <v>18</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L25" s="6" t="s">
         <v>23</v>
@@ -2526,7 +2523,7 @@
         <v>65</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>26</v>
@@ -2535,7 +2532,7 @@
         <v>16</v>
       </c>
       <c r="G26" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26" s="4">
         <v>5</v>
@@ -2547,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L26" s="6" t="s">
         <v>17</v>
@@ -2581,7 +2578,7 @@
         <v>68</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>26</v>
@@ -2602,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L27" s="6" t="s">
         <v>23</v>
@@ -2655,7 +2652,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L28" s="6" t="s">
         <v>17</v>
@@ -2708,7 +2705,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L29" s="6" t="s">
         <v>20</v>
@@ -2742,7 +2739,7 @@
         <v>75</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>15</v>
@@ -2763,7 +2760,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L30" s="6" t="s">
         <v>17</v>
@@ -2795,7 +2792,7 @@
         <v>77</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>15</v>
@@ -2816,7 +2813,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L31" s="6" t="s">
         <v>20</v>
@@ -2869,7 +2866,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L32" s="6" t="s">
         <v>17</v>
@@ -2922,7 +2919,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L33" s="6" t="s">
         <v>20</v>
@@ -2954,7 +2951,7 @@
         <v>83</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>15</v>
@@ -2975,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L34" s="6" t="s">
         <v>17</v>
@@ -3007,7 +3004,7 @@
         <v>85</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>15</v>
@@ -3028,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L35" s="6" t="s">
         <v>20</v>
@@ -3081,7 +3078,7 @@
         <v>0</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L36" s="6" t="s">
         <v>17</v>
@@ -3134,7 +3131,7 @@
         <v>0</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>20</v>
@@ -3187,7 +3184,7 @@
         <v>0</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L38" s="6" t="s">
         <v>17</v>
@@ -3240,7 +3237,7 @@
         <v>0</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>17</v>
@@ -3293,7 +3290,7 @@
         <v>0</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L40" s="6" t="s">
         <v>20</v>
@@ -3346,7 +3343,7 @@
         <v>0</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L41" s="6" t="s">
         <v>17</v>
@@ -3399,7 +3396,7 @@
         <v>0</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L42" s="6" t="s">
         <v>17</v>
@@ -3452,7 +3449,7 @@
         <v>0</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L43" s="6" t="s">
         <v>17</v>
@@ -3507,7 +3504,7 @@
         <v>0</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L44" s="6" t="s">
         <v>17</v>
@@ -3560,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L45" s="6" t="s">
         <v>17</v>
@@ -3613,7 +3610,7 @@
         <v>0</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L46" s="6" t="s">
         <v>17</v>
@@ -3666,7 +3663,7 @@
         <v>0</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L47" s="6" t="s">
         <v>20</v>

</xml_diff>